<commit_message>
upgrade import and export solution fr
</commit_message>
<xml_diff>
--- a/public/solicitud/prueba.xlsx
+++ b/public/solicitud/prueba.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID</t>
   </si>
@@ -35,53 +35,17 @@
     <t>GRADO</t>
   </si>
   <si>
-    <t>1-A</t>
-  </si>
-  <si>
-    <t>LEONIDAS RIOJA LIZARAZU</t>
-  </si>
-  <si>
-    <t>JULIO FRANCISCO NINA PATANI</t>
-  </si>
-  <si>
-    <t>2-A</t>
-  </si>
-  <si>
-    <t>3-A</t>
-  </si>
-  <si>
-    <t>ALEX REMBERTO GUTIERREZ GIRONDA</t>
-  </si>
-  <si>
-    <t>JULIO PINTO YUJRA</t>
-  </si>
-  <si>
-    <t>SEBASTIAN VILLCA APAZA</t>
-  </si>
-  <si>
-    <t>AGUSTIN MAMANI CHURA</t>
-  </si>
-  <si>
-    <t>JOSE DAVID MAMANI CONDORI</t>
-  </si>
-  <si>
-    <t>JESUS TOLA YUPANQUI</t>
-  </si>
-  <si>
     <t>NOMBRES</t>
   </si>
   <si>
-    <t>NICOLASA HUANTO VILLCA VDA. DE SIÑANI</t>
-  </si>
-  <si>
-    <t>CELIA MARIA ALI CHACHAQUE VDA. DE SALAS</t>
+    <t>RAMOS SANCHEZ JORGE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,13 +71,6 @@
       <color rgb="FF000000"/>
       <name val="Cantarell"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -135,7 +92,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -180,38 +137,16 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -221,14 +156,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -524,138 +453,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="4">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" thickBot="1">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="7"/>
+      <c r="D2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>